<commit_message>
Planteado la nueva forma de enviar reclamos
</commit_message>
<xml_diff>
--- a/plantillaPresentismo.xlsx
+++ b/plantillaPresentismo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20956852766\Desktop\Liquidacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\20956852766\Desktop\LIQ\liquidacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,14 +15,14 @@
     <sheet name="liquidacion" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">liquidacion!$A$6:$F$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">liquidacion!$A$7:$F$7</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Recuperadores</t>
+  </si>
+  <si>
+    <t>Pago de</t>
   </si>
 </sst>
 </file>
@@ -110,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -132,12 +135,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -169,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -222,11 +219,17 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +541,7 @@
       <c r="C2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="19"/>
+      <c r="D2" s="18"/>
       <c r="F2" s="16"/>
       <c r="G2" s="17" t="s">
         <v>10</v>
@@ -565,54 +568,61 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="C5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" s="14"/>
+      <c r="I6" s="20"/>
+    </row>
+    <row r="7" spans="1:9" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B7" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C7" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="18"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="7"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
@@ -727,6 +737,9 @@
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="10"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>